<commit_message>
for loop and some scrapping
</commit_message>
<xml_diff>
--- a/scrapping/pandas2day.xlsx
+++ b/scrapping/pandas2day.xlsx
@@ -501,18 +501,18 @@
       <c r="B4" t="inlineStr">
         <is>
           <t xml:space="preserve">
-ICICI Bank
+Olectra Greentech
 </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1062.70</t>
+          <t>2101.50</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1066.00</t>
+          <t>2221.95</t>
         </is>
       </c>
     </row>
@@ -523,18 +523,18 @@
       <c r="B5" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Olectra Greentech
+ICICI Bank
 </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2101.50</t>
+          <t>1062.70</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2221.95</t>
+          <t>1066.00</t>
         </is>
       </c>
     </row>
@@ -633,18 +633,18 @@
       <c r="B10" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Tata Invest Corp
+Bharat Electronics
 </t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>6977.50</t>
+          <t>194.75</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>7111.15</t>
+          <t>196.00</t>
         </is>
       </c>
     </row>
@@ -655,18 +655,18 @@
       <c r="B11" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Bharat Electronics
+Tata Invest Corp
 </t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>194.75</t>
+          <t>6977.50</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>196.00</t>
+          <t>7111.15</t>
         </is>
       </c>
     </row>

</xml_diff>